<commit_message>
Added changes to commitment spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/budget/effort_committment.xlsx
+++ b/docs/budget/effort_committment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-7000" yWindow="-28500" windowWidth="48580" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-5200" yWindow="-25440" windowWidth="48580" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,67 +562,7 @@
     <cellStyle name="Neutral" xfId="55" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1392,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1494,7 +1434,7 @@
       </c>
       <c r="C9" s="11"/>
       <c r="F9" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
@@ -1522,7 +1462,7 @@
       </c>
       <c r="F10" s="3">
         <f>$F$9+(C10*$C$3)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -1549,7 +1489,7 @@
       </c>
       <c r="F11" s="3">
         <f>$F$9+(C11*$C$3)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -1607,7 +1547,7 @@
       <c r="K17" s="24"/>
       <c r="L17" s="28">
         <f>SUM(E35:L37)</f>
-        <v>16.5</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="18" spans="2:32">
@@ -1627,7 +1567,7 @@
       <c r="K18" s="23"/>
       <c r="L18" s="27">
         <f>SUM(I35:L37)</f>
-        <v>16.5</v>
+        <v>23.5</v>
       </c>
       <c r="M18" s="21" t="s">
         <v>45</v>
@@ -1642,7 +1582,7 @@
       <c r="U18" s="21"/>
       <c r="V18" s="25">
         <f>SUM(M35:V37)</f>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="W18" s="22" t="s">
         <v>46</v>
@@ -1651,7 +1591,7 @@
       <c r="Y18" s="22"/>
       <c r="Z18" s="26">
         <f>SUM(W35:Z37)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:32">
@@ -1862,91 +1802,91 @@
         <v>20</v>
       </c>
       <c r="E23" s="4">
-        <f>$G$15 +($C$2  * (E$21-1))</f>
+        <f t="shared" ref="E23:Z23" si="1">$G$15 +($C$2  * (E$21-1))</f>
         <v>43031</v>
       </c>
       <c r="F23" s="4">
-        <f>$G$15 +($C$2  * (F$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43038</v>
       </c>
       <c r="G23" s="4">
-        <f>$G$15 +($C$2  * (G$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43045</v>
       </c>
       <c r="H23" s="4">
-        <f>$G$15 +($C$2  * (H$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43052</v>
       </c>
       <c r="I23" s="4">
-        <f>$G$15 +($C$2  * (I$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43059</v>
       </c>
       <c r="J23" s="4">
-        <f>$G$15 +($C$2  * (J$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43066</v>
       </c>
       <c r="K23" s="4">
-        <f>$G$15 +($C$2  * (K$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43073</v>
       </c>
       <c r="L23" s="4">
-        <f>$G$15 +($C$2  * (L$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43080</v>
       </c>
       <c r="M23" s="4">
-        <f>$G$15 +($C$2  * (M$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43087</v>
       </c>
       <c r="N23" s="4">
-        <f>$G$15 +($C$2  * (N$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43094</v>
       </c>
       <c r="O23" s="4">
-        <f>$G$15 +($C$2  * (O$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43101</v>
       </c>
       <c r="P23" s="4">
-        <f>$G$15 +($C$2  * (P$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43108</v>
       </c>
       <c r="Q23" s="4">
-        <f>$G$15 +($C$2  * (Q$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43115</v>
       </c>
       <c r="R23" s="4">
-        <f>$G$15 +($C$2  * (R$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43122</v>
       </c>
       <c r="S23" s="4">
-        <f>$G$15 +($C$2  * (S$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43129</v>
       </c>
       <c r="T23" s="4">
-        <f>$G$15 +($C$2  * (T$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43136</v>
       </c>
       <c r="U23" s="4">
-        <f>$G$15 +($C$2  * (U$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43143</v>
       </c>
       <c r="V23" s="4">
-        <f>$G$15 +($C$2  * (V$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43150</v>
       </c>
       <c r="W23" s="4">
-        <f>$G$15 +($C$2  * (W$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43157</v>
       </c>
       <c r="X23" s="4">
-        <f>$G$15 +($C$2  * (X$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43164</v>
       </c>
       <c r="Y23" s="4">
-        <f>$G$15 +($C$2  * (Y$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43171</v>
       </c>
       <c r="Z23" s="4">
-        <f>$G$15 +($C$2  * (Z$21-1))</f>
+        <f t="shared" si="1"/>
         <v>43178</v>
       </c>
       <c r="AC23" s="5" t="str">
@@ -2036,20 +1976,20 @@
         <v>12</v>
       </c>
       <c r="AC24" s="3">
-        <f t="shared" ref="AC24:AC33" si="1">COUNTIFS($E24:$AB24,$I$9) * $F$9</f>
-        <v>28</v>
+        <f t="shared" ref="AC24:AC33" si="2">COUNTIFS($E24:$AB24,$I$9) * $F$9</f>
+        <v>42</v>
       </c>
       <c r="AD24" s="3">
-        <f t="shared" ref="AD24:AD33" si="2">COUNTIFS($E24:$AB24,$I$10) * $F$10</f>
-        <v>4.5</v>
+        <f t="shared" ref="AD24:AD33" si="3">COUNTIFS($E24:$AB24,$I$10) * $F$10</f>
+        <v>5.5</v>
       </c>
       <c r="AE24" s="3">
-        <f t="shared" ref="AE24:AE33" si="3">COUNTIFS($E24:$AB24,$I$11) * $F$11</f>
+        <f t="shared" ref="AE24:AE33" si="4">COUNTIFS($E24:$AB24,$I$11) * $F$11</f>
         <v>0</v>
       </c>
       <c r="AF24" s="3">
-        <f t="shared" ref="AF24:AF33" si="4">SUM(AC24:AE24)</f>
-        <v>32.5</v>
+        <f t="shared" ref="AF24:AF33" si="5">SUM(AC24:AE24)</f>
+        <v>47.5</v>
       </c>
     </row>
     <row r="25" spans="2:32">
@@ -2123,20 +2063,20 @@
         <v>12</v>
       </c>
       <c r="AC25" s="3">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
       <c r="AD25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF25" s="3">
-        <f t="shared" si="4"/>
-        <v>28</v>
+        <f t="shared" si="5"/>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="2:32">
@@ -2210,19 +2150,19 @@
         <v>31</v>
       </c>
       <c r="AC26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF26" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2297,19 +2237,19 @@
         <v>31</v>
       </c>
       <c r="AC27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF27" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2384,19 +2324,19 @@
         <v>31</v>
       </c>
       <c r="AC28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2471,19 +2411,19 @@
         <v>31</v>
       </c>
       <c r="AC29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF29" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2558,19 +2498,19 @@
         <v>31</v>
       </c>
       <c r="AC30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2645,19 +2585,19 @@
         <v>31</v>
       </c>
       <c r="AC31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2732,19 +2672,19 @@
         <v>31</v>
       </c>
       <c r="AC32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2819,19 +2759,19 @@
         <v>31</v>
       </c>
       <c r="AC33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2847,92 +2787,92 @@
         <v>Minimum</v>
       </c>
       <c r="E35" s="3">
-        <f>COUNTIFS(E$24:E$34,$I9) * $F$9</f>
+        <f t="shared" ref="E35:Z35" si="6">COUNTIFS(E$24:E$34,$I9) * $F$9</f>
         <v>0</v>
       </c>
       <c r="F35" s="3">
-        <f>COUNTIFS(F$24:F$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G35" s="3">
-        <f>COUNTIFS(G$24:G$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H35" s="3">
-        <f>COUNTIFS(H$24:H$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I35" s="3">
-        <f>COUNTIFS(I$24:I$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J35" s="3">
-        <f>COUNTIFS(J$24:J$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="K35" s="3">
-        <f>COUNTIFS(K$24:K$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="L35" s="3">
-        <f>COUNTIFS(L$24:L$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="M35" s="3">
-        <f>COUNTIFS(M$24:M$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N35" s="3">
-        <f>COUNTIFS(N$24:N$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O35" s="3">
-        <f>COUNTIFS(O$24:O$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P35" s="3">
-        <f>COUNTIFS(P$24:P$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="Q35" s="3">
-        <f>COUNTIFS(Q$24:Q$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="R35" s="3">
-        <f>COUNTIFS(R$24:R$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="S35" s="3">
-        <f>COUNTIFS(S$24:S$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="T35" s="3">
-        <f>COUNTIFS(T$24:T$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="U35" s="3">
-        <f>COUNTIFS(U$24:U$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="V35" s="3">
-        <f>COUNTIFS(V$24:V$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="W35" s="3">
-        <f>COUNTIFS(W$24:W$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="X35" s="3">
-        <f>COUNTIFS(X$24:X$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="Y35" s="3">
-        <f>COUNTIFS(Y$24:Y$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="Z35" s="3">
-        <f>COUNTIFS(Z$24:Z$34,$I9) * $F$9</f>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:33" s="3" customFormat="1">
@@ -2942,91 +2882,91 @@
         <v>Expected</v>
       </c>
       <c r="E36" s="3">
-        <f>COUNTIFS(E$24:E$34,$I10) * $F$10</f>
+        <f t="shared" ref="E36:Z36" si="7">COUNTIFS(E$24:E$34,$I10) * $F$10</f>
         <v>0</v>
       </c>
       <c r="F36" s="3">
-        <f>COUNTIFS(F$24:F$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G36" s="3">
-        <f>COUNTIFS(G$24:G$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H36" s="3">
-        <f>COUNTIFS(H$24:H$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I36" s="3">
-        <f>COUNTIFS(I$24:I$34,$I10) * $F$10</f>
-        <v>4.5</v>
+        <f t="shared" si="7"/>
+        <v>5.5</v>
       </c>
       <c r="J36" s="3">
-        <f>COUNTIFS(J$24:J$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K36" s="3">
-        <f>COUNTIFS(K$24:K$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L36" s="3">
-        <f>COUNTIFS(L$24:L$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M36" s="3">
-        <f>COUNTIFS(M$24:M$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N36" s="3">
-        <f>COUNTIFS(N$24:N$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O36" s="3">
-        <f>COUNTIFS(O$24:O$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P36" s="3">
-        <f>COUNTIFS(P$24:P$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q36" s="3">
-        <f>COUNTIFS(Q$24:Q$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R36" s="3">
-        <f>COUNTIFS(R$24:R$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S36" s="3">
-        <f>COUNTIFS(S$24:S$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T36" s="3">
-        <f>COUNTIFS(T$24:T$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U36" s="3">
-        <f>COUNTIFS(U$24:U$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V36" s="3">
-        <f>COUNTIFS(V$24:V$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W36" s="3">
-        <f>COUNTIFS(W$24:W$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X36" s="3">
-        <f>COUNTIFS(X$24:X$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y36" s="3">
-        <f>COUNTIFS(Y$24:Y$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z36" s="3">
-        <f>COUNTIFS(Z$24:Z$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB36" s="5" t="s">
@@ -3034,11 +2974,11 @@
       </c>
       <c r="AC36" s="5">
         <f>SUM(AC24:AC34)</f>
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="AD36" s="5">
         <f>SUM(AD24:AD34)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="AE36" s="5">
         <f>SUM(AE24:AE34)</f>
@@ -3046,7 +2986,7 @@
       </c>
       <c r="AF36" s="5">
         <f>SUM(AF24:AF34)</f>
-        <v>60.5</v>
+        <v>89.5</v>
       </c>
       <c r="AG36" s="5" t="s">
         <v>5</v>
@@ -3059,91 +2999,91 @@
         <v>Stretch</v>
       </c>
       <c r="E37" s="3">
-        <f>COUNTIFS(E$24:E$34,$I11) * $F$11</f>
+        <f t="shared" ref="E37:Z37" si="8">COUNTIFS(E$24:E$34,$I11) * $F$11</f>
         <v>0</v>
       </c>
       <c r="F37" s="3">
-        <f>COUNTIFS(F$24:F$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G37" s="3">
-        <f>COUNTIFS(G$24:G$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H37" s="3">
-        <f>COUNTIFS(H$24:H$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I37" s="3">
-        <f>COUNTIFS(I$24:I$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J37" s="3">
-        <f>COUNTIFS(J$24:J$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K37" s="3">
-        <f>COUNTIFS(K$24:K$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L37" s="3">
-        <f>COUNTIFS(L$24:L$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M37" s="3">
-        <f>COUNTIFS(M$24:M$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N37" s="3">
-        <f>COUNTIFS(N$24:N$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O37" s="3">
-        <f>COUNTIFS(O$24:O$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P37" s="3">
-        <f>COUNTIFS(P$24:P$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q37" s="3">
-        <f>COUNTIFS(Q$24:Q$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R37" s="3">
-        <f>COUNTIFS(R$24:R$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S37" s="3">
-        <f>COUNTIFS(S$24:S$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T37" s="3">
-        <f>COUNTIFS(T$24:T$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U37" s="3">
-        <f>COUNTIFS(U$24:U$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V37" s="3">
-        <f>COUNTIFS(V$24:V$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W37" s="3">
-        <f>COUNTIFS(W$24:W$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X37" s="3">
-        <f>COUNTIFS(X$24:X$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y37" s="3">
-        <f>COUNTIFS(Y$24:Y$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z37" s="3">
-        <f>COUNTIFS(Z$24:Z$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3171,92 +3111,92 @@
         <v>19</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" ref="E42:Z42" si="5">SUM(E35:E37)</f>
+        <f t="shared" ref="E42:Z42" si="9">SUM(E35:E37)</f>
         <v>0</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="5"/>
-        <v>4.5</v>
+        <f t="shared" si="9"/>
+        <v>5.5</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="L42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="Q42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="R42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="T42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="U42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="V42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="W42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="X42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="Y42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="Z42" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="AB42" s="5" t="s">
         <v>26</v>
@@ -3265,7 +3205,7 @@
       <c r="AD42" s="5"/>
       <c r="AE42" s="5">
         <f>SUM(E42:Z42)</f>
-        <v>60.5</v>
+        <v>89.5</v>
       </c>
       <c r="AF42" s="5"/>
       <c r="AG42" s="5" t="s">
@@ -3284,44 +3224,44 @@
         <v>0</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" ref="H43:Z43" si="6">SUM(G42:H42)</f>
+        <f t="shared" ref="H43:Z43" si="10">SUM(G42:H42)</f>
         <v>0</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="6"/>
-        <v>8.5</v>
+        <f t="shared" si="10"/>
+        <v>11.5</v>
       </c>
       <c r="L43" s="3">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>12</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P43" s="3">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>6</v>
       </c>
       <c r="R43" s="3">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>12</v>
       </c>
       <c r="T43" s="3">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>12</v>
       </c>
       <c r="V43" s="3">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>12</v>
       </c>
       <c r="X43" s="3">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>12</v>
       </c>
       <c r="Z43" s="3">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>12</v>
       </c>
       <c r="AB43" s="5" t="s">
         <v>26</v>
@@ -3330,7 +3270,7 @@
       <c r="AD43" s="5"/>
       <c r="AE43" s="5">
         <f>SUM(D43:Z43)</f>
-        <v>60.5</v>
+        <v>89.5</v>
       </c>
       <c r="AG43" s="5" t="s">
         <v>5</v>
@@ -3342,7 +3282,7 @@
       </c>
       <c r="C47" s="7">
         <f>AE43</f>
-        <v>60.5</v>
+        <v>89.5</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>33</v>
@@ -3350,207 +3290,207 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AF34:AF35 A32:B32 D32 AA32:XFD32">
-    <cfRule type="cellIs" dxfId="49" priority="132" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="132" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="133" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="133" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="134" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="134" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:XFD20">
-    <cfRule type="cellIs" dxfId="46" priority="130" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="130" operator="between">
       <formula>$K$10</formula>
       <formula>$K$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="131" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="131" operator="between">
       <formula>$K$9</formula>
       <formula>$K$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:Z37">
-    <cfRule type="cellIs" dxfId="44" priority="127" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="127" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="128" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="128" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="129" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="129" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:D24 C25:C32 AA24:XFD24">
-    <cfRule type="cellIs" dxfId="41" priority="124" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="124" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="125" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="125" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="126" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="126" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:B25 D25 AA25:XFD25">
-    <cfRule type="cellIs" dxfId="38" priority="121" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="121" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="122" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="122" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="123" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="123" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26 D26 AA26:XFD26">
-    <cfRule type="cellIs" dxfId="35" priority="118" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="118" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="119" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="119" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="120" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="120" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B31 D31 AA31:XFD31">
-    <cfRule type="cellIs" dxfId="32" priority="100" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="100" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="101" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="101" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="102" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="102" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27 D27 AA27:XFD27">
-    <cfRule type="cellIs" dxfId="29" priority="112" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="112" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="113" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="113" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="114" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="114" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B28 D28 AA28:XFD28">
-    <cfRule type="cellIs" dxfId="26" priority="109" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="109" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="110" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="110" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="111" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="111" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:B29 D29 AA29:XFD29">
-    <cfRule type="cellIs" dxfId="23" priority="106" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="106" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="107" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="107" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="108" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="108" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30 D30 AA30:XFD30">
-    <cfRule type="cellIs" dxfId="20" priority="103" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="103" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="104" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="104" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="105" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="105" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33 D33 AA33:XFD33">
-    <cfRule type="cellIs" dxfId="17" priority="97" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="97" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="98" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="98" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="99" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="99" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="14" priority="94" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="94" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="95" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="95" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="96" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="96" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24:Z25">
-    <cfRule type="cellIs" dxfId="11" priority="82" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="82" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="83" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="83" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="84" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="84" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:O25 E26:Z33">
-    <cfRule type="cellIs" dxfId="8" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="43" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="44" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="44" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="45" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="45" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>

</xml_diff>